<commit_message>
improved conformance tests; added type checking on setattr
</commit_message>
<xml_diff>
--- a/tests/util/conformance/metadata1.xlsx
+++ b/tests/util/conformance/metadata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sect1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>is_primary</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>sect1 description</t>
+  </si>
+  <si>
+    <t>in</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -165,8 +167,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -180,13 +186,17 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,7 +528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -564,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -645,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>